<commit_message>
temp changed and random fixed
</commit_message>
<xml_diff>
--- a/src/assets/template/SIDON - example file.xlsx
+++ b/src/assets/template/SIDON - example file.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Muminniyoz\BMI-2022\dasturlar\umb-front\src\assets\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A56717A-9406-48A1-944B-957FFA37C903}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9D3EF6A-8B56-4485-94EF-7EFB10F7C867}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="shablon" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="35">
   <si>
     <t>&lt;1-alomat tur&gt;</t>
   </si>
@@ -125,6 +125,18 @@
   </si>
   <si>
     <t>Lobar Mamatova</t>
+  </si>
+  <si>
+    <t>Soch rangi</t>
+  </si>
+  <si>
+    <t>qora</t>
+  </si>
+  <si>
+    <t>qong'ir</t>
+  </si>
+  <si>
+    <t>sariq</t>
   </si>
 </sst>
 </file>
@@ -632,20 +644,20 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" style="2" customWidth="1"/>
-    <col min="2" max="2" width="25.21875" style="2" customWidth="1"/>
-    <col min="3" max="4" width="18.77734375" style="2" customWidth="1"/>
-    <col min="5" max="5" width="15.77734375" style="2" customWidth="1"/>
-    <col min="6" max="6" width="14.77734375" style="2" customWidth="1"/>
+    <col min="1" max="1" width="8.90625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="25.1796875" style="2" customWidth="1"/>
+    <col min="3" max="4" width="18.81640625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="15.81640625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="14.81640625" style="2" customWidth="1"/>
     <col min="7" max="7" width="18" style="2" customWidth="1"/>
-    <col min="8" max="9" width="8.88671875" style="2"/>
-    <col min="10" max="10" width="47.77734375" style="2" customWidth="1"/>
-    <col min="11" max="16384" width="8.88671875" style="2"/>
+    <col min="8" max="9" width="8.90625" style="2"/>
+    <col min="10" max="10" width="47.81640625" style="2" customWidth="1"/>
+    <col min="11" max="16384" width="8.90625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="8" t="s">
         <v>18</v>
       </c>
@@ -673,7 +685,7 @@
       <c r="K1" s="10"/>
       <c r="L1" s="10"/>
     </row>
-    <row r="2" spans="1:12" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="8" t="s">
         <v>20</v>
       </c>
@@ -701,7 +713,7 @@
       <c r="K2" s="10"/>
       <c r="L2" s="10"/>
     </row>
-    <row r="3" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -719,7 +731,7 @@
       <c r="K3" s="10"/>
       <c r="L3" s="10"/>
     </row>
-    <row r="4" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -737,7 +749,7 @@
       <c r="K4" s="10"/>
       <c r="L4" s="10"/>
     </row>
-    <row r="5" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -755,7 +767,7 @@
       <c r="K5" s="10"/>
       <c r="L5" s="10"/>
     </row>
-    <row r="6" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -773,7 +785,7 @@
       <c r="K6" s="10"/>
       <c r="L6" s="10"/>
     </row>
-    <row r="7" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -791,7 +803,7 @@
       <c r="K7" s="10"/>
       <c r="L7" s="10"/>
     </row>
-    <row r="8" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -806,7 +818,7 @@
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
     </row>
-    <row r="9" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -821,34 +833,34 @@
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B11" s="12" t="s">
         <v>23</v>
       </c>
       <c r="C11" s="13"/>
       <c r="D11" s="14"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B12" s="15"/>
       <c r="C12" s="16"/>
       <c r="D12" s="17"/>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B13" s="15"/>
       <c r="C13" s="16"/>
       <c r="D13" s="17"/>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B14" s="15"/>
       <c r="C14" s="16"/>
       <c r="D14" s="17"/>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B15" s="15"/>
       <c r="C15" s="16"/>
       <c r="D15" s="17"/>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B16" s="18"/>
       <c r="C16" s="19"/>
       <c r="D16" s="20"/>
@@ -863,23 +875,23 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3585ABB-FB59-44E1-9385-07DF58D8FF8C}">
-  <dimension ref="A1:H9"/>
+  <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="3" width="22.44140625" customWidth="1"/>
-    <col min="4" max="4" width="20" customWidth="1"/>
-    <col min="5" max="5" width="20.6640625" customWidth="1"/>
-    <col min="6" max="6" width="20.88671875" customWidth="1"/>
-    <col min="7" max="7" width="18.109375" customWidth="1"/>
-    <col min="8" max="8" width="19" customWidth="1"/>
+    <col min="2" max="3" width="22.453125" customWidth="1"/>
+    <col min="4" max="5" width="20" customWidth="1"/>
+    <col min="6" max="6" width="20.6328125" customWidth="1"/>
+    <col min="7" max="7" width="20.90625" customWidth="1"/>
+    <col min="8" max="8" width="18.08984375" customWidth="1"/>
+    <col min="9" max="9" width="19" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" s="7" t="s">
         <v>18</v>
       </c>
@@ -893,19 +905,22 @@
         <v>1</v>
       </c>
       <c r="E1" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F1" s="3">
         <v>1</v>
       </c>
-      <c r="G1" s="5">
+      <c r="G1" s="3">
         <v>1</v>
       </c>
-      <c r="H1" s="11">
+      <c r="H1" s="5">
+        <v>1</v>
+      </c>
+      <c r="I1" s="11">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="8" t="s">
         <v>17</v>
       </c>
@@ -919,19 +934,22 @@
         <v>11</v>
       </c>
       <c r="E2" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="F2" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="G2" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="H2" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="H2" s="8" t="s">
+      <c r="I2" s="8" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -944,20 +962,23 @@
       <c r="D3" s="6">
         <v>0.56000000000000005</v>
       </c>
-      <c r="E3" s="1">
+      <c r="E3" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="F3" s="1">
         <v>70.599999999999994</v>
       </c>
-      <c r="F3" s="1">
+      <c r="G3" s="1">
         <v>19</v>
       </c>
-      <c r="G3" s="1">
+      <c r="H3" s="1">
         <v>178</v>
       </c>
-      <c r="H3" s="1">
+      <c r="I3" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -970,20 +991,23 @@
       <c r="D4" s="6">
         <v>0.96</v>
       </c>
-      <c r="E4" s="1">
+      <c r="E4" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="F4" s="1">
         <v>65</v>
       </c>
-      <c r="F4" s="1">
+      <c r="G4" s="1">
         <v>18</v>
       </c>
-      <c r="G4" s="1">
+      <c r="H4" s="1">
         <v>165</v>
       </c>
-      <c r="H4" s="1">
+      <c r="I4" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -996,20 +1020,23 @@
       <c r="D5" s="6">
         <v>0.56000000000000005</v>
       </c>
-      <c r="E5" s="1">
+      <c r="E5" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="F5" s="1">
         <v>84.5</v>
       </c>
-      <c r="F5" s="1">
+      <c r="G5" s="1">
         <v>17</v>
       </c>
-      <c r="G5" s="1">
+      <c r="H5" s="1">
         <v>145</v>
       </c>
-      <c r="H5" s="1">
+      <c r="I5" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -1022,20 +1049,23 @@
       <c r="D6" s="6">
         <v>0.85</v>
       </c>
-      <c r="E6" s="1">
+      <c r="E6" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="F6" s="1">
         <v>65</v>
       </c>
-      <c r="F6" s="1">
+      <c r="G6" s="1">
         <v>24</v>
       </c>
-      <c r="G6" s="1">
+      <c r="H6" s="1">
         <v>176</v>
       </c>
-      <c r="H6" s="1">
+      <c r="I6" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -1048,20 +1078,23 @@
       <c r="D7" s="6">
         <v>0.59</v>
       </c>
-      <c r="E7" s="1">
+      <c r="E7" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="F7" s="1">
         <v>50</v>
       </c>
-      <c r="F7" s="1">
+      <c r="G7" s="1">
         <v>21</v>
       </c>
-      <c r="G7" s="1">
+      <c r="H7" s="1">
         <v>160</v>
       </c>
-      <c r="H7" s="1">
+      <c r="I7" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -1074,20 +1107,23 @@
       <c r="D8" s="6">
         <v>0.78</v>
       </c>
-      <c r="E8" s="1">
+      <c r="E8" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="F8" s="1">
         <v>60</v>
       </c>
-      <c r="F8" s="1">
+      <c r="G8" s="1">
         <v>20</v>
       </c>
-      <c r="G8" s="1">
+      <c r="H8" s="1">
         <v>166</v>
       </c>
-      <c r="H8" s="1">
+      <c r="I8" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -1100,16 +1136,19 @@
       <c r="D9" s="6">
         <v>0.71</v>
       </c>
-      <c r="E9" s="1">
+      <c r="E9" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="F9" s="1">
         <v>68</v>
       </c>
-      <c r="F9" s="1">
+      <c r="G9" s="1">
         <v>24</v>
       </c>
-      <c r="G9" s="1">
+      <c r="H9" s="1">
         <v>170</v>
       </c>
-      <c r="H9" s="1">
+      <c r="I9" s="1">
         <v>2</v>
       </c>
     </row>

</xml_diff>